<commit_message>
update cards with resources and buildings
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -3,26 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633875D9-9408-4267-8BB0-0A8F56BE5D54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51819D3C-45F3-4BFD-95CB-27A59075F575}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
-    <sheet name="map tiles" sheetId="2" r:id="rId2"/>
+    <sheet name="map_tiles" sheetId="2" r:id="rId2"/>
     <sheet name="resources" sheetId="5" r:id="rId3"/>
     <sheet name="buildings" sheetId="6" r:id="rId4"/>
     <sheet name="event_cards" sheetId="3" r:id="rId5"/>
     <sheet name="player_cards" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="buildable">'map tiles'!$D$2:$D$10</definedName>
-    <definedName name="buildable_big">'map tiles'!$E$2:$E$10</definedName>
-    <definedName name="direct_water_source">'map tiles'!$G$2:$G$10</definedName>
-    <definedName name="names">'map tiles'!$B$2:$B$10</definedName>
-    <definedName name="number">'map tiles'!$C$2:$C$10</definedName>
-    <definedName name="traversable">'map tiles'!$F$2:$F$10</definedName>
-    <definedName name="underground_water_source">'map tiles'!$H$2:$H$10</definedName>
+    <definedName name="buildable">map_tiles!$D$2:$D$10</definedName>
+    <definedName name="buildable_big">map_tiles!$E$2:$E$10</definedName>
+    <definedName name="direct_water_source">map_tiles!$G$2:$G$10</definedName>
+    <definedName name="names">map_tiles!$B$2:$B$10</definedName>
+    <definedName name="number">map_tiles!$C$2:$C$10</definedName>
+    <definedName name="traversable">map_tiles!$F$2:$F$10</definedName>
+    <definedName name="underground_water_source">map_tiles!$H$2:$H$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="114">
   <si>
     <t>Map tiles</t>
   </si>
@@ -376,9 +376,6 @@
     <t>Snow storm</t>
   </si>
   <si>
-    <t>You find 3+2S of resource X, if you have at least one active scavenger, where S is the number of scavengers</t>
-  </si>
-  <si>
     <t>Sunny day</t>
   </si>
   <si>
@@ -397,21 +394,12 @@
     <t>Bridge</t>
   </si>
   <si>
-    <t>You found a bridge! Place it over a river</t>
-  </si>
-  <si>
-    <t>You found a building(1-6)! Place it in whichever building (not necessarily yours) or tile you want</t>
-  </si>
-  <si>
     <t>Subbuilding</t>
   </si>
   <si>
     <t>Building</t>
   </si>
   <si>
-    <t>You found a building(7-10)! Place it in whichever valid tile you want</t>
-  </si>
-  <si>
     <t>rate</t>
   </si>
   <si>
@@ -419,6 +407,9 @@
   </si>
   <si>
     <t>Every player gets 3 water</t>
+  </si>
+  <si>
+    <t>You found a BRIDGE! Place it over a river</t>
   </si>
 </sst>
 </file>
@@ -972,7 +963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1023,7 +1014,7 @@
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2395,7 +2386,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2411,7 +2402,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -2468,7 +2459,7 @@
         <v>0.1</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -2479,14 +2470,14 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="32">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -2497,14 +2488,14 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D6" s="32">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="E6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2515,14 +2506,14 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D7" s="32">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -2535,15 +2526,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25AADA5A-4821-472E-9CD2-9892448B123E}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2554,32 +2545,32 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="33">
         <v>1</v>
       </c>
       <c r="B2">
-        <f>8*5</f>
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>92</v>
       </c>
       <c r="D2" s="32">
         <f>B2/SUM(B:B)</f>
-        <v>0.52631578947368418</v>
-      </c>
-      <c r="E2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>6.5789473684210523E-2</v>
+      </c>
+      <c r="E2" t="str">
+        <f>_xlfn.CONCAT("You find ",UPPER(resources!B2),"! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger")</f>
+        <v>You find WATER! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="33">
         <v>2</v>
       </c>
@@ -2587,92 +2578,383 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" s="32">
-        <f t="shared" ref="D3:D7" si="0">B3/SUM(B:B)</f>
+        <f>B3/SUM(B:B)</f>
         <v>6.5789473684210523E-2</v>
       </c>
-      <c r="E3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E3" t="str">
+        <f>_xlfn.CONCAT("You find ",UPPER(resources!B3),"! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger")</f>
+        <v>You find FOOD! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="33">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D4" s="32">
-        <f t="shared" si="0"/>
-        <v>3.9473684210526314E-2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" ref="D4:D9" si="0">B4/SUM(B:B)</f>
+        <v>6.5789473684210523E-2</v>
+      </c>
+      <c r="E4" t="str">
+        <f>_xlfn.CONCAT("You find ",UPPER(resources!B4),"! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger")</f>
+        <v>You find MEDICINES! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="33">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="D5" s="32">
         <f t="shared" si="0"/>
-        <v>0.15789473684210525</v>
-      </c>
-      <c r="E5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>6.5789473684210523E-2</v>
+      </c>
+      <c r="E5" t="str">
+        <f>_xlfn.CONCAT("You find ",UPPER(resources!B5),"! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger")</f>
+        <v>You find ROCK! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="33">
         <v>5</v>
       </c>
       <c r="B6">
-        <f>6*2</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="D6" s="32">
         <f t="shared" si="0"/>
-        <v>0.15789473684210525</v>
-      </c>
-      <c r="E6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>6.5789473684210523E-2</v>
+      </c>
+      <c r="E6" t="str">
+        <f>_xlfn.CONCAT("You find ",UPPER(resources!B6),"! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger")</f>
+        <v>You find WOOD! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="33">
         <v>6</v>
       </c>
       <c r="B7">
-        <f>4*1</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D7" s="32">
         <f t="shared" si="0"/>
-        <v>5.2631578947368418E-2</v>
-      </c>
-      <c r="E7" t="s">
+        <v>6.5789473684210523E-2</v>
+      </c>
+      <c r="E7" t="str">
+        <f>_xlfn.CONCAT("You find ",UPPER(resources!B7),"! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger")</f>
+        <v>You find TOOLS! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="33">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="32">
+        <f t="shared" si="0"/>
+        <v>6.5789473684210523E-2</v>
+      </c>
+      <c r="E8" t="str">
+        <f>_xlfn.CONCAT("You find ",UPPER(resources!B8),"! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger")</f>
+        <v>You find WEAPONS! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="33">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="32">
+        <f t="shared" si="0"/>
+        <v>6.5789473684210523E-2</v>
+      </c>
+      <c r="E9" t="str">
+        <f>_xlfn.CONCAT("You find ",UPPER(resources!B9),"! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger")</f>
+        <v>You find INFORMATION! You get 3+2S, where S is the number of scavengers, if you have at least one active scavenger</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="33">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="32">
+        <f>B10/SUM(B:B)</f>
+        <v>6.5789473684210523E-2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="33">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="32">
+        <f>B11/SUM(B:B)</f>
+        <v>3.9473684210526314E-2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="33">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="32">
+        <f>B12/SUM(B:B)</f>
+        <v>0.15789473684210525</v>
+      </c>
+      <c r="E12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P11" s="32"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="33">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="32">
+        <f>B13/SUM(B:B)</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E13" t="str">
+        <f>_xlfn.CONCAT("You found a ", UPPER(buildings!B3),"! Place it in whichever building (not necessarily yours) or tile you want")</f>
+        <v>You found a WELL! Place it in whichever building (not necessarily yours) or tile you want</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="33">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="32">
+        <f>B14/SUM(B:B)</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E14" t="str">
+        <f>_xlfn.CONCAT("You found a ", UPPER(buildings!B4),"! Place it in whichever building (not necessarily yours) or tile you want")</f>
+        <v>You found a WATER CLEANER! Place it in whichever building (not necessarily yours) or tile you want</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="33">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="32">
+        <f t="shared" ref="D15:D20" si="1">B15/SUM(B:B)</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E15" t="str">
+        <f>_xlfn.CONCAT("You found a ", UPPER(buildings!B5),"! Place it in whichever building (not necessarily yours) or tile you want")</f>
+        <v>You found a FARMACY! Place it in whichever building (not necessarily yours) or tile you want</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="33">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="32">
+        <f t="shared" si="1"/>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E16" t="str">
+        <f>_xlfn.CONCAT("You found a ", UPPER(buildings!B6),"! Place it in whichever building (not necessarily yours) or tile you want")</f>
+        <v>You found a WORKSHOP! Place it in whichever building (not necessarily yours) or tile you want</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="33">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="32">
+        <f t="shared" si="1"/>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E17" t="str">
+        <f>_xlfn.CONCAT("You found a ", UPPER(buildings!B7),"! Place it in whichever building (not necessarily yours) or tile you want")</f>
+        <v>You found a RADIO STATION! Place it in whichever building (not necessarily yours) or tile you want</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="33">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="32">
+        <f t="shared" si="1"/>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E18" t="str">
+        <f>_xlfn.CONCAT("You found a ", UPPER(buildings!B8),"! Place it in whichever building (not necessarily yours) or tile you want")</f>
+        <v>You found a WATCH TOWER! Place it in whichever building (not necessarily yours) or tile you want</v>
+      </c>
+      <c r="P18" s="32"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="33">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="32">
+        <f t="shared" si="1"/>
+        <v>1.3157894736842105E-2</v>
+      </c>
+      <c r="E19" t="str">
+        <f>_xlfn.CONCAT("You found a ", UPPER(buildings!B9),"! Place it in whichever building (not necessarily yours) or tile you want")</f>
+        <v>You found a FARM! Place it in whichever building (not necessarily yours) or tile you want</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="33">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="32">
+        <f t="shared" si="1"/>
+        <v>1.3157894736842105E-2</v>
+      </c>
+      <c r="E20" t="str">
+        <f>_xlfn.CONCAT("You found a ", UPPER(buildings!B10),"! Place it in whichever building (not necessarily yours) or tile you want")</f>
+        <v>You found a HUNTER CAMP! Place it in whichever building (not necessarily yours) or tile you want</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="33">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="32">
+        <f t="shared" ref="D21:D24" si="2">B21/SUM(B:B)</f>
+        <v>1.3157894736842105E-2</v>
+      </c>
+      <c r="E21" t="str">
+        <f>_xlfn.CONCAT("You found a ", UPPER(buildings!B11),"! Place it in whichever building (not necessarily yours) or tile you want")</f>
+        <v>You found a LUMBER CAMP! Place it in whichever building (not necessarily yours) or tile you want</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="33">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="32">
+        <f t="shared" si="2"/>
+        <v>1.3157894736842105E-2</v>
+      </c>
+      <c r="E22" t="str">
+        <f>_xlfn.CONCAT("You found a ", UPPER(buildings!B12),"! Place it in whichever building (not necessarily yours) or tile you want")</f>
+        <v>You found a QUARRY! Place it in whichever building (not necessarily yours) or tile you want</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="33"/>
+      <c r="D23" s="32"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="33"/>
+      <c r="D24" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
basic game over xlsx
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51819D3C-45F3-4BFD-95CB-27A59075F575}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471112A2-C3B7-4A50-84A3-1DD6061904CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -964,7 +964,7 @@
   <dimension ref="B2:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1014,7 +1014,7 @@
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1620,7 +1620,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1787,7 +1787,7 @@
   <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2921,7 +2921,7 @@
         <v>109</v>
       </c>
       <c r="D21" s="32">
-        <f t="shared" ref="D21:D24" si="2">B21/SUM(B:B)</f>
+        <f t="shared" ref="D21:D22" si="2">B21/SUM(B:B)</f>
         <v>1.3157894736842105E-2</v>
       </c>
       <c r="E21" t="str">

</xml_diff>

<commit_message>
add icons for the map
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471112A2-C3B7-4A50-84A3-1DD6061904CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92181E53-445A-4A70-930A-7B48578F55DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -963,7 +963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -1786,8 +1786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5531790B-02F5-4EEF-93DC-68D09484BB8E}">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>